<commit_message>
awners & maintaince cars
</commit_message>
<xml_diff>
--- a/public/files/cars/cars-export.xlsx
+++ b/public/files/cars/cars-export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,51 @@
     <t>Tipo de Servicio</t>
   </si>
   <si>
+    <t>Número Interno</t>
+  </si>
+  <si>
+    <t>Tipo de Relación</t>
+  </si>
+  <si>
+    <t>Cilindraje</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>Tipo de Carrocería</t>
+  </si>
+  <si>
+    <t>Número de Puertas</t>
+  </si>
+  <si>
+    <t>Número de Motor</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Número de serie</t>
+  </si>
+  <si>
+    <t>Toneladas Carga</t>
+  </si>
+  <si>
+    <t>Número de Chasis</t>
+  </si>
+  <si>
+    <t>Fecha de Matricula</t>
+  </si>
+  <si>
+    <t>Kilometros para cambio de aceite</t>
+  </si>
+  <si>
+    <t>Propietario</t>
+  </si>
+  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -50,54 +95,69 @@
     <t>VMX324</t>
   </si>
   <si>
-    <t>Chevrolet</t>
+    <t>CHEVROLET</t>
   </si>
   <si>
     <t>Diesel Premium</t>
   </si>
   <si>
-    <t>QP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transporte </t>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transporte Especial </t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>CAMIONETA</t>
+  </si>
+  <si>
+    <t>TSS547</t>
+  </si>
+  <si>
+    <t>RANGER</t>
+  </si>
+  <si>
+    <t>GUQ918</t>
+  </si>
+  <si>
+    <t>GEV101</t>
+  </si>
+  <si>
+    <t>BUSETA</t>
+  </si>
+  <si>
+    <t>SXD370</t>
+  </si>
+  <si>
+    <t>TSS520</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
+  </si>
+  <si>
+    <t>HILUX</t>
+  </si>
+  <si>
+    <t>TSS518</t>
+  </si>
+  <si>
+    <t>TSS552</t>
   </si>
   <si>
     <t>Inactivo</t>
   </si>
   <si>
-    <t>CAMIONETA</t>
-  </si>
-  <si>
-    <t>TSS547</t>
-  </si>
-  <si>
-    <t>Activo</t>
-  </si>
-  <si>
-    <t>GUQ918</t>
-  </si>
-  <si>
-    <t>GEV101</t>
-  </si>
-  <si>
-    <t>BUSETA</t>
-  </si>
-  <si>
-    <t>SXD370</t>
-  </si>
-  <si>
-    <t>TSS520</t>
-  </si>
-  <si>
-    <t>TSS518</t>
-  </si>
-  <si>
-    <t>TSS552</t>
-  </si>
-  <si>
     <t>GEU189</t>
   </si>
   <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>ALASKAN</t>
+  </si>
+  <si>
     <t>GEV031</t>
   </si>
   <si>
@@ -171,6 +231,36 @@
   </si>
   <si>
     <t>THW212</t>
+  </si>
+  <si>
+    <t>XTQ999</t>
+  </si>
+  <si>
+    <t>VHX324</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>CCC000</t>
+  </si>
+  <si>
+    <t>VEHÍCULO AFILIADO</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>PARTICULAR</t>
+  </si>
+  <si>
+    <t>desconocida</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>mario</t>
   </si>
 </sst>
 </file>
@@ -509,7 +599,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +607,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,66 +635,149 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1991</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>2020</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>2019</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>2020</v>
@@ -613,19 +786,34 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>2020</v>
@@ -634,19 +822,34 @@
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>2019</v>
@@ -655,40 +858,78 @@
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>2019</v>
       </c>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>2019</v>
@@ -697,103 +938,210 @@
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>2019</v>
       </c>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>2019</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>2020</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>2020</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
-        <v>2019</v>
-      </c>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D12">
-        <v>2019</v>
-      </c>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>2020</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <v>2019</v>
@@ -802,19 +1150,34 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
-      <c r="I13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>2019</v>
@@ -823,19 +1186,34 @@
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>2019</v>
@@ -844,19 +1222,34 @@
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D16">
         <v>2019</v>
@@ -865,19 +1258,34 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="I16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>2019</v>
@@ -886,19 +1294,34 @@
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
-      <c r="I17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D18">
         <v>2019</v>
@@ -907,19 +1330,34 @@
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
-      <c r="I18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D19">
         <v>2019</v>
@@ -928,19 +1366,34 @@
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
-      <c r="I19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>2019</v>
@@ -949,19 +1402,34 @@
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D21">
         <v>2019</v>
@@ -970,19 +1438,34 @@
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D22">
         <v>2019</v>
@@ -991,19 +1474,34 @@
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
-      <c r="I22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>2019</v>
@@ -1012,19 +1510,34 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
-      <c r="I23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>2019</v>
@@ -1033,19 +1546,34 @@
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>
-      <c r="I24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>2019</v>
@@ -1054,19 +1582,34 @@
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>2019</v>
@@ -1075,19 +1618,34 @@
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
-      <c r="I26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D27">
         <v>2019</v>
@@ -1096,19 +1654,34 @@
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
-      <c r="I27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D28">
         <v>2019</v>
@@ -1117,19 +1690,34 @@
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
-      <c r="I28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D29">
         <v>2019</v>
@@ -1138,19 +1726,34 @@
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
-      <c r="I29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>2019</v>
@@ -1159,19 +1762,34 @@
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
-      <c r="I30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D31">
         <v>2019</v>
@@ -1180,19 +1798,34 @@
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31"/>
-      <c r="I31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D32">
         <v>2019</v>
@@ -1201,19 +1834,34 @@
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
-      <c r="I32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33">
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D33">
         <v>2019</v>
@@ -1222,19 +1870,34 @@
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
-      <c r="I33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34">
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D34">
         <v>2019</v>
@@ -1243,19 +1906,34 @@
       <c r="F34"/>
       <c r="G34"/>
       <c r="H34"/>
-      <c r="I34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35">
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D35">
         <v>2019</v>
@@ -1264,8 +1942,185 @@
       <c r="F35"/>
       <c r="G35"/>
       <c r="H35"/>
-      <c r="I35" t="s">
-        <v>18</v>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36">
+        <v>2019</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>2001</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>1901</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38" t="s">
+        <v>76</v>
+      </c>
+      <c r="K38">
+        <v>1200</v>
+      </c>
+      <c r="L38" t="s">
+        <v>77</v>
+      </c>
+      <c r="M38" t="s">
+        <v>78</v>
+      </c>
+      <c r="N38" t="s">
+        <v>79</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38">
+        <v>267890</v>
+      </c>
+      <c r="Q38">
+        <v>100</v>
+      </c>
+      <c r="R38">
+        <v>4567890</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1876567</v>
+      </c>
+      <c r="U38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V38">
+        <v>5000</v>
+      </c>
+      <c r="W38" t="s">
+        <v>81</v>
+      </c>
+      <c r="X38" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>